<commit_message>
update: progress final revision
</commit_message>
<xml_diff>
--- a/public/assets/format/FORMAT IMPORT BARANG.xlsx
+++ b/public/assets/format/FORMAT IMPORT BARANG.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtio\OneDrive - PT MRT JAKARTA\Documents\WEB\ukt2\public\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtio\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{65434FA9-1DDA-4D4F-B29C-3E421981FA61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{18801F5A-E8B0-4781-8FB5-756BE924DE0A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033933E3-A760-4D43-A6F2-59EB1689BB63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{FB1DBD40-E52F-4CBF-8CFD-392A65E13483}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TUTORIAL PENGISIAN" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -117,16 +118,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -165,19 +193,68 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>162935</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814305D8-1238-44BC-A641-7DE079511C5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="38100"/>
+          <a:ext cx="7240010" cy="2152950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEA1BB3B-16B6-4535-83C5-CC8DF8D72800}" name="Table1" displayName="Table1" ref="A1:I3" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEA1BB3B-16B6-4535-83C5-CC8DF8D72800}" name="Table1" displayName="Table1" ref="A1:I3" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:I3" xr:uid="{03619000-BB1D-4422-91EA-88203AC2CC33}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{53E0C5D4-AD71-4160-B046-F80C8F1B1541}" name="Nama"/>
     <tableColumn id="2" xr3:uid="{9B5768CB-FD41-488A-ABE7-5D0D92DE636A}" name="Kode"/>
     <tableColumn id="3" xr3:uid="{76784594-F9A4-414A-9B0B-4A6FAF554F52}" name="Merk"/>
     <tableColumn id="4" xr3:uid="{B5AF9FD6-9D8B-4BD1-BC12-88E9C1C1B29F}" name="Jenis"/>
-    <tableColumn id="5" xr3:uid="{201858B1-424B-42C3-91D8-ADDAA8B147F4}" name="Stock awal"/>
-    <tableColumn id="6" xr3:uid="{287494CC-308F-415F-AE70-2FED73FDB5EE}" name="Stock aktual"/>
-    <tableColumn id="7" xr3:uid="{ED71E077-E538-4D41-9FD9-A600FDF883B3}" name="Satuan"/>
+    <tableColumn id="5" xr3:uid="{201858B1-424B-42C3-91D8-ADDAA8B147F4}" name="Stock awal" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{287494CC-308F-415F-AE70-2FED73FDB5EE}" name="Stock aktual" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{ED71E077-E538-4D41-9FD9-A600FDF883B3}" name="Satuan" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{1B1ED142-8B09-473C-B403-9FFBA6F245D1}" name="Harga"/>
-    <tableColumn id="9" xr3:uid="{14B4E70C-A981-4DD5-B65B-8F249DE222CE}" name="Spesifikasi"/>
+    <tableColumn id="9" xr3:uid="{14B4E70C-A981-4DD5-B65B-8F249DE222CE}" name="Spesifikasi" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -483,20 +560,24 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="91.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -524,7 +605,7 @@
       <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -541,19 +622,19 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>17</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H2">
         <v>78000</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -570,27 +651,52 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H3">
         <v>15000</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{418837CE-75CA-4D61-B077-D10AB3DADBB7}">
+      <formula1>"consumable, tools,"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432A8A86-2B0D-4242-8688-67C9C467D19B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="84.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>